<commit_message>
Added input jack switching circuits, fab files updated and finalized.
</commit_message>
<xml_diff>
--- a/Echo Cinematic/FAB FILES - Echo Cinematic/BOM - Echo Cinematic.xlsx
+++ b/Echo Cinematic/FAB FILES - Echo Cinematic/BOM - Echo Cinematic.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Supul Sapukotana\Desktop\Dropbox\Fiverr\Clients\jasonmayo898\Echo Cinematic\FAB FILES - Echo Cinematic\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Supul Sapukotana\Documents\GitHub\EchoCinematic-hw\Echo Cinematic\FAB FILES - Echo Cinematic\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="149">
   <si>
     <t>Footprint</t>
   </si>
@@ -216,9 +216,6 @@
     <t>0R</t>
   </si>
   <si>
-    <t>R19, R28</t>
-  </si>
-  <si>
     <t>R20, R23</t>
   </si>
   <si>
@@ -312,15 +309,6 @@
     <t>Multiplier</t>
   </si>
   <si>
-    <t>U1</t>
-  </si>
-  <si>
-    <t>ES_DAISY_SEED2_DFM</t>
-  </si>
-  <si>
-    <t>FOOTPRINTS:DAISY_SEED2</t>
-  </si>
-  <si>
     <t>U2, U8</t>
   </si>
   <si>
@@ -393,9 +381,6 @@
     <t>SMD,P=1.27mm</t>
   </si>
   <si>
-    <t>C59983</t>
-  </si>
-  <si>
     <t>C1017</t>
   </si>
   <si>
@@ -475,6 +460,12 @@
   </si>
   <si>
     <t>C423022</t>
+  </si>
+  <si>
+    <t>R19, R28, R51, R52</t>
+  </si>
+  <si>
+    <t>C3975131</t>
   </si>
 </sst>
 </file>
@@ -1285,10 +1276,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F52"/>
+  <dimension ref="A1:F51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+      <selection activeCell="A49" sqref="A49:XFD49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1302,22 +1293,22 @@
   <sheetData>
     <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1334,7 +1325,7 @@
         <v>805</v>
       </c>
       <c r="E2" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1351,7 +1342,7 @@
         <v>603</v>
       </c>
       <c r="E3" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1368,7 +1359,7 @@
         <v>603</v>
       </c>
       <c r="E4" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1385,7 +1376,7 @@
         <v>603</v>
       </c>
       <c r="E5" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1402,7 +1393,7 @@
         <v>603</v>
       </c>
       <c r="E6" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1416,10 +1407,10 @@
         <v>3</v>
       </c>
       <c r="D7" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="E7" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1436,7 +1427,7 @@
         <v>603</v>
       </c>
       <c r="E8" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1447,13 +1438,13 @@
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D9" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="E9" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1484,10 +1475,10 @@
         <v>20</v>
       </c>
       <c r="D11" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="E11" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -1501,10 +1492,10 @@
         <v>22</v>
       </c>
       <c r="D12" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="E12" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -1515,7 +1506,7 @@
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="D13" t="s">
         <v>24</v>
@@ -1532,7 +1523,7 @@
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D14" t="s">
         <v>24</v>
@@ -1634,13 +1625,13 @@
         <v>5</v>
       </c>
       <c r="C20" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="D20" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="E20" t="s">
-        <v>124</v>
+        <v>148</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -1674,7 +1665,7 @@
         <v>805</v>
       </c>
       <c r="E22" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -1691,7 +1682,7 @@
         <v>44</v>
       </c>
       <c r="E23" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -1708,7 +1699,7 @@
         <v>603</v>
       </c>
       <c r="E24" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -1725,7 +1716,7 @@
         <v>603</v>
       </c>
       <c r="E25" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -1742,7 +1733,7 @@
         <v>603</v>
       </c>
       <c r="E26" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -1759,7 +1750,7 @@
         <v>603</v>
       </c>
       <c r="E27" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -1776,7 +1767,7 @@
         <v>603</v>
       </c>
       <c r="E28" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -1793,7 +1784,7 @@
         <v>603</v>
       </c>
       <c r="E29" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -1810,7 +1801,7 @@
         <v>603</v>
       </c>
       <c r="E30" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -1827,7 +1818,7 @@
         <v>603</v>
       </c>
       <c r="E31" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -1844,7 +1835,7 @@
         <v>603</v>
       </c>
       <c r="E32" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -1861,15 +1852,15 @@
         <v>805</v>
       </c>
       <c r="E33" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>65</v>
+        <v>147</v>
       </c>
       <c r="B34">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C34" t="s">
         <v>64</v>
@@ -1878,80 +1869,80 @@
         <v>603</v>
       </c>
       <c r="E34" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B35">
         <v>2</v>
       </c>
       <c r="C35" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D35">
         <v>603</v>
       </c>
       <c r="E35" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B36">
         <v>2</v>
       </c>
       <c r="C36" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D36">
         <v>603</v>
       </c>
       <c r="E36" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>69</v>
+      </c>
+      <c r="B37">
+        <v>1</v>
+      </c>
+      <c r="C37" t="s">
         <v>70</v>
-      </c>
-      <c r="B37">
-        <v>1</v>
-      </c>
-      <c r="C37" t="s">
-        <v>71</v>
       </c>
       <c r="D37">
         <v>603</v>
       </c>
       <c r="E37" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B38">
         <v>4</v>
       </c>
       <c r="C38" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D38">
         <v>603</v>
       </c>
       <c r="E38" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B39">
         <v>7</v>
@@ -1960,7 +1951,7 @@
         <v>54</v>
       </c>
       <c r="D39" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E39" t="s">
         <v>1</v>
@@ -1968,7 +1959,7 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B40">
         <v>3</v>
@@ -1977,7 +1968,7 @@
         <v>54</v>
       </c>
       <c r="D40" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E40" t="s">
         <v>1</v>
@@ -1985,16 +1976,16 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>77</v>
+      </c>
+      <c r="B41">
+        <v>1</v>
+      </c>
+      <c r="C41" t="s">
         <v>78</v>
       </c>
-      <c r="B41">
-        <v>1</v>
-      </c>
-      <c r="C41" t="s">
+      <c r="D41" t="s">
         <v>79</v>
-      </c>
-      <c r="D41" t="s">
-        <v>80</v>
       </c>
       <c r="E41" t="s">
         <v>1</v>
@@ -2002,16 +1993,16 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
+        <v>80</v>
+      </c>
+      <c r="B42">
+        <v>1</v>
+      </c>
+      <c r="C42" t="s">
         <v>81</v>
       </c>
-      <c r="B42">
-        <v>1</v>
-      </c>
-      <c r="C42" t="s">
-        <v>82</v>
-      </c>
       <c r="D42" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E42" t="s">
         <v>1</v>
@@ -2019,16 +2010,16 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
+        <v>82</v>
+      </c>
+      <c r="B43">
+        <v>1</v>
+      </c>
+      <c r="C43" t="s">
         <v>83</v>
       </c>
-      <c r="B43">
-        <v>1</v>
-      </c>
-      <c r="C43" t="s">
+      <c r="D43" t="s">
         <v>84</v>
-      </c>
-      <c r="D43" t="s">
-        <v>85</v>
       </c>
       <c r="E43" t="s">
         <v>1</v>
@@ -2036,16 +2027,16 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
+        <v>85</v>
+      </c>
+      <c r="B44">
+        <v>1</v>
+      </c>
+      <c r="C44" t="s">
         <v>86</v>
       </c>
-      <c r="B44">
-        <v>1</v>
-      </c>
-      <c r="C44" t="s">
+      <c r="D44" t="s">
         <v>87</v>
-      </c>
-      <c r="D44" t="s">
-        <v>88</v>
       </c>
       <c r="E44" t="s">
         <v>1</v>
@@ -2053,16 +2044,16 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
+        <v>88</v>
+      </c>
+      <c r="B45">
+        <v>1</v>
+      </c>
+      <c r="C45" t="s">
         <v>89</v>
       </c>
-      <c r="B45">
-        <v>1</v>
-      </c>
-      <c r="C45" t="s">
-        <v>90</v>
-      </c>
       <c r="D45" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E45" t="s">
         <v>1</v>
@@ -2070,16 +2061,16 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
+        <v>90</v>
+      </c>
+      <c r="B46">
+        <v>1</v>
+      </c>
+      <c r="C46" t="s">
         <v>91</v>
       </c>
-      <c r="B46">
-        <v>1</v>
-      </c>
-      <c r="C46" t="s">
-        <v>92</v>
-      </c>
       <c r="D46" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E46" t="s">
         <v>1</v>
@@ -2087,16 +2078,16 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
+        <v>92</v>
+      </c>
+      <c r="B47">
+        <v>1</v>
+      </c>
+      <c r="C47" t="s">
         <v>93</v>
       </c>
-      <c r="B47">
-        <v>1</v>
-      </c>
-      <c r="C47" t="s">
-        <v>94</v>
-      </c>
       <c r="D47" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E47" t="s">
         <v>1</v>
@@ -2104,16 +2095,16 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
+        <v>94</v>
+      </c>
+      <c r="B48">
+        <v>1</v>
+      </c>
+      <c r="C48" t="s">
         <v>95</v>
       </c>
-      <c r="B48">
-        <v>1</v>
-      </c>
-      <c r="C48" t="s">
-        <v>96</v>
-      </c>
       <c r="D48" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E48" t="s">
         <v>1</v>
@@ -2121,70 +2112,53 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
+        <v>96</v>
+      </c>
+      <c r="B49">
+        <v>2</v>
+      </c>
+      <c r="C49" t="s">
         <v>97</v>
       </c>
-      <c r="B49">
-        <v>1</v>
-      </c>
-      <c r="C49" t="s">
-        <v>98</v>
-      </c>
       <c r="D49" t="s">
-        <v>99</v>
+        <v>135</v>
       </c>
       <c r="E49" t="s">
-        <v>1</v>
+        <v>136</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B50">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C50" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D50" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="E50" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B51">
         <v>1</v>
       </c>
       <c r="C51" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D51" t="s">
-        <v>140</v>
+        <v>44</v>
       </c>
       <c r="E51" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>104</v>
-      </c>
-      <c r="B52">
-        <v>1</v>
-      </c>
-      <c r="C52" t="s">
-        <v>105</v>
-      </c>
-      <c r="D52" t="s">
-        <v>44</v>
-      </c>
-      <c r="E52" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>

</xml_diff>